<commit_message>
Implement DuckDuckGo search engine test cases
</commit_message>
<xml_diff>
--- a/build/resources/test/testData.xlsx
+++ b/build/resources/test/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\JavaProjects\AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11622887-8E22-4765-9166-85343CA20367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6960E85-CACE-4FF8-9C7E-C1DEC43D9DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="780" windowWidth="18570" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="780" windowWidth="18570" windowHeight="15030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Google" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Keyword</t>
   </si>
@@ -34,13 +34,19 @@
     <t>ethical hacking</t>
   </si>
   <si>
+    <t>automation testing</t>
+  </si>
+  <si>
+    <t>quality assurance</t>
+  </si>
+  <si>
+    <t>ruby is the best programming language</t>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
     <t>hire me please</t>
-  </si>
-  <si>
-    <t>privacy</t>
-  </si>
-  <si>
-    <t>no such element exception selenium</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +420,16 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -427,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3382F67F-ED1F-46F2-A7C5-A9668D7828C3}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,12 +464,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug in logCommonResults() method inside SharedMethods.java class
</commit_message>
<xml_diff>
--- a/build/resources/test/testData.xlsx
+++ b/build/resources/test/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\JavaProjects\AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC53EC38-5240-48DF-B375-038850AC6C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C19668-DC74-4049-988D-7A2D97306EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="780" windowWidth="18570" windowHeight="15030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Keyword</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>privacy</t>
-  </si>
-  <si>
-    <t>hire me please</t>
   </si>
 </sst>
 </file>
@@ -405,7 +402,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,12 +441,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -469,7 +466,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change filtering common results by website title instead of urls
</commit_message>
<xml_diff>
--- a/build/resources/test/testData.xlsx
+++ b/build/resources/test/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\JavaProjects\AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C19668-DC74-4049-988D-7A2D97306EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73118C3C-9461-4725-85B1-EAD35098B0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="780" windowWidth="18570" windowHeight="15030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Keyword</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>ethical hacking</t>
-  </si>
-  <si>
-    <t>privacy</t>
   </si>
 </sst>
 </file>
@@ -402,7 +399,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +438,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +458,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>